<commit_message>
feat: added translation from latest delta
</commit_message>
<xml_diff>
--- a/utils/localization/resources/Bhasha_Daan_All_Content_July_16.xlsx
+++ b/utils/localization/resources/Bhasha_Daan_All_Content_July_16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localization/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8847A575-C6BF-B04B-9CB5-6D9EA35EE026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F64321-87B2-034B-ACEA-2A95642EC3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16174,9 +16174,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A413" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A171" sqref="A171"/>
+      <selection pane="topRight" activeCell="A439" sqref="A439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>